<commit_message>
docs(experiments-data): Updating Experiment 1 plot
- Removing log-scale from Experiment 1 plot so we can see the xticks.
</commit_message>
<xml_diff>
--- a/files/experiments/SchalaDB-Experiments-2021.xlsx
+++ b/files/experiments/SchalaDB-Experiments-2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/Google Drive/DBox@GDrive/Doctorate/2017/MINHA-DAPD-Journal/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EABAE9-CD34-D048-8366-0F45FC02FFC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA6E53A-C908-4D40-A864-8701F4DA3677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34880" windowHeight="20240" xr2:uid="{73171AA7-8BB2-984F-9F98-F4EAD9BE95F5}"/>
+    <workbookView xWindow="10720" yWindow="780" windowWidth="26860" windowHeight="20220" xr2:uid="{73171AA7-8BB2-984F-9F98-F4EAD9BE95F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong scalability" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,6 @@
     <sheet name="OLAP queries" sheetId="10" r:id="rId7"/>
     <sheet name="d-Chiron vs. Chiron" sheetId="13" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,16 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
-  <si>
-    <t>12 threads</t>
-  </si>
-  <si>
-    <t>24 threads</t>
-  </si>
-  <si>
-    <t>48 threads</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Cores</t>
   </si>
@@ -280,6 +267,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB39E85"/>
+      <color rgb="FFAA967D"/>
+      <color rgb="FF947666"/>
+      <color rgb="FF945200"/>
+      <color rgb="FFF49E96"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -337,7 +333,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -358,7 +354,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$C$4:$C$7</c:f>
+              <c:f>'Strong scalability'!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -410,7 +406,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -431,7 +427,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$E$4:$E$7</c:f>
+              <c:f>'Strong scalability'!$E$3:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -466,9 +462,7 @@
           <c:spPr>
             <a:ln w="25400">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:srgbClr val="945200"/>
               </a:solidFill>
               <a:prstDash val="dashDot"/>
             </a:ln>
@@ -476,9 +470,7 @@
           <c:marker>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:srgbClr val="945200"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -487,7 +479,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -508,7 +500,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$G$4:$G$7</c:f>
+              <c:f>'Strong scalability'!$G$3:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -543,10 +535,7 @@
           <c:spPr>
             <a:ln w="12700">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="F49E96"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -563,7 +552,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -584,7 +573,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$I$4:$I$7</c:f>
+              <c:f>'Strong scalability'!$I$3:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -619,25 +608,29 @@
           <c:spPr>
             <a:ln w="12700">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8F9A-6D4F-AD97-552E75DF3FD2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -658,7 +651,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$J$4:$J$7</c:f>
+              <c:f>'Strong scalability'!$J$3:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -693,7 +686,7 @@
           <c:spPr>
             <a:ln w="12700">
               <a:solidFill>
-                <a:srgbClr val="CEA041"/>
+                <a:srgbClr val="B39E85"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -707,7 +700,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$A$4:$A$7</c:f>
+              <c:f>'Strong scalability'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -728,7 +721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong scalability'!$K$4:$K$7</c:f>
+              <c:f>'Strong scalability'!$K$3:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -768,7 +761,6 @@
       <c:valAx>
         <c:axId val="529593312"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
           <c:min val="100"/>
@@ -803,7 +795,8 @@
         <c:crossAx val="529596704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="100"/>
+        <c:minorUnit val="100"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="529596704"/>
@@ -844,7 +837,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="529593312"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="100"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -6474,13 +6467,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>271123</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>66592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>411502</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>157930</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6512,13 +6505,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>194040</xdr:colOff>
-      <xdr:row>162</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>167000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>204120</xdr:colOff>
-      <xdr:row>162</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>172400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -7115,458 +7108,6 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Plan1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Plan2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="N2" t="str">
-            <v>12 threads</v>
-          </cell>
-          <cell r="R2" t="str">
-            <v>24 threads</v>
-          </cell>
-          <cell r="V2" t="str">
-            <v>48 threads</v>
-          </cell>
-          <cell r="Z2" t="str">
-            <v>Linear</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="M4">
-            <v>120</v>
-          </cell>
-          <cell r="Q4">
-            <v>1</v>
-          </cell>
-          <cell r="U4">
-            <v>1</v>
-          </cell>
-          <cell r="Y4">
-            <v>1</v>
-          </cell>
-          <cell r="Z4">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="M5">
-            <v>240</v>
-          </cell>
-          <cell r="Q5">
-            <v>1.9799999999999998</v>
-          </cell>
-          <cell r="U5">
-            <v>1.9286396633511445</v>
-          </cell>
-          <cell r="Y5">
-            <v>1.8560599849255244</v>
-          </cell>
-          <cell r="Z5">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="M6">
-            <v>480</v>
-          </cell>
-          <cell r="Q6">
-            <v>3.8176086886715783</v>
-          </cell>
-          <cell r="U6">
-            <v>3.6251196597170861</v>
-          </cell>
-          <cell r="Y6">
-            <v>3.28046919078125</v>
-          </cell>
-          <cell r="Z6">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="M7">
-            <v>960</v>
-          </cell>
-          <cell r="Q7">
-            <v>7.1724666322691899</v>
-          </cell>
-          <cell r="U7">
-            <v>6.3495052292512923</v>
-          </cell>
-          <cell r="Y7">
-            <v>5.3521867806642547</v>
-          </cell>
-          <cell r="Z7">
-            <v>8</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="I1" t="str">
-            <v># tasks</v>
-          </cell>
-          <cell r="N1" t="str">
-            <v>Ideal</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>Expected Time</v>
-          </cell>
-          <cell r="U1" t="str">
-            <v>Exec. Time</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="D2">
-            <v>240</v>
-          </cell>
-          <cell r="I2">
-            <v>6.0019999999999998</v>
-          </cell>
-          <cell r="N2">
-            <v>29.160083333333333</v>
-          </cell>
-          <cell r="U2">
-            <v>29.160083333333333</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3">
-            <v>480</v>
-          </cell>
-          <cell r="I3">
-            <v>12.002000000000001</v>
-          </cell>
-          <cell r="N3">
-            <v>29.160083333333333</v>
-          </cell>
-          <cell r="U3">
-            <v>32.731649999999995</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>936</v>
-          </cell>
-          <cell r="I4">
-            <v>23.402000000000001</v>
-          </cell>
-          <cell r="N4">
-            <v>29.160083333333333</v>
-          </cell>
-          <cell r="U4">
-            <v>39.642716666666665</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>5</v>
-          </cell>
-          <cell r="N8">
-            <v>0.57309583333333336</v>
-          </cell>
-          <cell r="Q8">
-            <v>3.1194999999999999</v>
-          </cell>
-          <cell r="U8">
-            <v>3.1194999999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>30</v>
-          </cell>
-          <cell r="N9">
-            <v>3.4385750000000002</v>
-          </cell>
-          <cell r="Q9">
-            <v>18.716999999999999</v>
-          </cell>
-          <cell r="U9">
-            <v>5.2169166666666662</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>60</v>
-          </cell>
-          <cell r="N10">
-            <v>6.8771500000000003</v>
-          </cell>
-          <cell r="Q10">
-            <v>62.602999999999994</v>
-          </cell>
-          <cell r="U10">
-            <v>7.7842833333333337</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>120</v>
-          </cell>
-          <cell r="N11">
-            <v>13.754300000000001</v>
-          </cell>
-          <cell r="Q11">
-            <v>186.8228</v>
-          </cell>
-          <cell r="U11">
-            <v>13.754300000000001</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>5</v>
-          </cell>
-          <cell r="N14">
-            <v>2.6335562499999998</v>
-          </cell>
-          <cell r="Q14">
-            <v>16.580233333333332</v>
-          </cell>
-          <cell r="U14">
-            <v>16.580233333333332</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>30</v>
-          </cell>
-          <cell r="N15">
-            <v>15.801337500000001</v>
-          </cell>
-          <cell r="Q15">
-            <v>99.481399999999994</v>
-          </cell>
-          <cell r="U15">
-            <v>27.004650000000002</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>60</v>
-          </cell>
-          <cell r="N16">
-            <v>31.602675000000001</v>
-          </cell>
-          <cell r="Q16">
-            <v>324.05580000000003</v>
-          </cell>
-          <cell r="U16">
-            <v>39.642716666666665</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>120</v>
-          </cell>
-          <cell r="N17">
-            <v>63.205350000000003</v>
-          </cell>
-          <cell r="Q17">
-            <v>951.4251999999999</v>
-          </cell>
-          <cell r="U17">
-            <v>63.205350000000003</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="K20">
-            <v>1</v>
-          </cell>
-          <cell r="N20">
-            <v>7.7842833333333337</v>
-          </cell>
-          <cell r="U20">
-            <v>7.7842833333333337</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="K21">
-            <v>0.98846437599555559</v>
-          </cell>
-          <cell r="N21">
-            <v>20.233816353410223</v>
-          </cell>
-          <cell r="U21">
-            <v>20.469949999999997</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="K22">
-            <v>0.9814694641308781</v>
-          </cell>
-          <cell r="N22">
-            <v>38.908115883525561</v>
-          </cell>
-          <cell r="U22">
-            <v>39.642716666666665</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="K26">
-            <v>1</v>
-          </cell>
-          <cell r="N26">
-            <v>3.1194999999999999</v>
-          </cell>
-          <cell r="U26">
-            <v>3.1194999999999999</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="K27">
-            <v>0.97319570635560504</v>
-          </cell>
-          <cell r="N27">
-            <v>8.1085679196924385</v>
-          </cell>
-          <cell r="U27">
-            <v>8.3318985757316657</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="K28">
-            <v>0.9404071393786837</v>
-          </cell>
-          <cell r="N28">
-            <v>15.592169799231097</v>
-          </cell>
-          <cell r="U28">
-            <v>16.580233333333332</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="N32">
-            <v>8.6999999999999993</v>
-          </cell>
-          <cell r="U32">
-            <v>8.6999999999999993</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="N33">
-            <v>17.397100966344549</v>
-          </cell>
-          <cell r="U33">
-            <v>15.23</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="N34">
-            <v>33.921592802399196</v>
-          </cell>
-          <cell r="U34">
-            <v>27.36</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="C196" t="str">
-            <v>Workload: 23k tasks, 5s on average</v>
-          </cell>
-          <cell r="D196" t="str">
-            <v>4k tasks, 120s on average</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="C197">
-            <v>17.02</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="C198">
-            <v>16.580233333333332</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Plan1"/>
-      <sheetName val="Scalability-SparkVsChiron"/>
-      <sheetName val="ActivityCost-SparkvsDChiron"/>
-      <sheetName val="dChironVSChiron"/>
-      <sheetName val="HIL"/>
-      <sheetName val="DDDBMSBottlenecks"/>
-      <sheetName val="DBMS1s"/>
-      <sheetName val="DBMS16s"/>
-      <sheetName val="DBMS60s"/>
-      <sheetName val="DDBMSSchedBottleneck"/>
-      <sheetName val="Plan3"/>
-      <sheetName val="DDBMS.Sched."/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>5k tasks, 1 s</v>
-          </cell>
-          <cell r="C17" t="str">
-            <v>5 k, tasks 16 s</v>
-          </cell>
-          <cell r="D17" t="str">
-            <v>20 k, tasks 1 s</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>20 k tasks, 16 s</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>d-Chiron</v>
-          </cell>
-          <cell r="B18">
-            <v>4.9578499999999996</v>
-          </cell>
-          <cell r="C18">
-            <v>9.4707666669999995</v>
-          </cell>
-          <cell r="D18">
-            <v>5.5125833330000003</v>
-          </cell>
-          <cell r="E18">
-            <v>9.5169499999999996</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Chiron</v>
-          </cell>
-          <cell r="B19">
-            <v>11.36838333</v>
-          </cell>
-          <cell r="C19">
-            <v>11.654716669999999</v>
-          </cell>
-          <cell r="D19">
-            <v>61.49271667</v>
-          </cell>
-          <cell r="E19">
-            <v>63.167050000000003</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10121,10 +9662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02AA410-21FC-F547-AF9C-39BDE2FF8EE5}">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="69" zoomScalePageLayoutView="113" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="69" zoomScalePageLayoutView="113" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10143,251 +9684,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="7" t="str">
+        <f>"12 threads"</f>
+        <v>12 threads</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="str">
+        <f>"24 threads"</f>
+        <v>24 threads</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="str">
+        <f>"48 threads"</f>
+        <v>48 threads</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="7" t="str">
-        <f>"12 threads"</f>
-        <v>12 threads</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="str">
-        <f>"24 threads"</f>
-        <v>24 threads</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="str">
-        <f>"48 threads"</f>
-        <v>48 threads</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>7</v>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3">
+        <v>17001.105659999997</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/60</f>
+        <v>283.35176099999995</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8592.4869999999992</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3/60</f>
+        <v>143.20811666666665</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4459.6239999999998</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/60</f>
+        <v>74.327066666666667</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <f>C3</f>
+        <v>283.35176099999995</v>
+      </c>
+      <c r="J3" s="1">
+        <f>E3</f>
+        <v>143.20811666666665</v>
+      </c>
+      <c r="K3" s="1">
+        <f>G3</f>
+        <v>74.327066666666667</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B4" s="3">
-        <v>17001.105659999997</v>
+        <v>8586.4169999999995</v>
       </c>
       <c r="C4" s="3">
         <f>B4/60</f>
-        <v>283.35176099999995</v>
+        <v>143.10694999999998</v>
       </c>
       <c r="D4" s="3">
-        <v>8592.4869999999992</v>
+        <v>4455.2060000000001</v>
       </c>
       <c r="E4" s="3">
         <f>D4/60</f>
-        <v>143.20811666666665</v>
+        <v>74.253433333333334</v>
       </c>
       <c r="F4" s="3">
-        <v>4459.6239999999998</v>
+        <v>2402.7370000000001</v>
       </c>
       <c r="G4" s="3">
         <f>F4/60</f>
-        <v>74.327066666666667</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1</v>
+        <v>40.045616666666668</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
       </c>
       <c r="I4" s="1">
-        <f>C4</f>
-        <v>283.35176099999995</v>
+        <f>C3/H4</f>
+        <v>141.67588049999998</v>
       </c>
       <c r="J4" s="1">
-        <f>E4</f>
-        <v>143.20811666666665</v>
+        <f>E3/H4</f>
+        <v>71.604058333333327</v>
       </c>
       <c r="K4" s="1">
-        <f>G4</f>
-        <v>74.327066666666667</v>
+        <f>G3/H4</f>
+        <v>37.163533333333334</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="B5" s="3">
-        <v>8586.4169999999995</v>
+        <v>4453.3389999999999</v>
       </c>
       <c r="C5" s="3">
         <f>B5/60</f>
-        <v>143.10694999999998</v>
+        <v>74.222316666666671</v>
       </c>
       <c r="D5" s="3">
-        <v>4455.2060000000001</v>
+        <v>2370.2629999999999</v>
       </c>
       <c r="E5" s="3">
         <f>D5/60</f>
-        <v>74.253433333333334</v>
+        <v>39.50438333333333</v>
       </c>
       <c r="F5" s="3">
-        <v>2402.7370000000001</v>
+        <v>1359.4469999999999</v>
       </c>
       <c r="G5" s="3">
         <f>F5/60</f>
-        <v>40.045616666666668</v>
+        <v>22.657449999999997</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1">
-        <f>C4/H5</f>
-        <v>141.67588049999998</v>
+        <f>C3/H5</f>
+        <v>70.837940249999988</v>
       </c>
       <c r="J5" s="1">
-        <f>E4/H5</f>
-        <v>71.604058333333327</v>
+        <f>E3/H5</f>
+        <v>35.802029166666664</v>
       </c>
       <c r="K5" s="1">
-        <f>G4/H5</f>
-        <v>37.163533333333334</v>
+        <f>G3/H5</f>
+        <v>18.581766666666667</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="B6" s="3">
-        <v>4453.3389999999999</v>
+        <v>2370.3290000000002</v>
       </c>
       <c r="C6" s="3">
         <f>B6/60</f>
-        <v>74.222316666666671</v>
+        <v>39.505483333333338</v>
       </c>
       <c r="D6" s="3">
-        <v>2370.2629999999999</v>
+        <v>1353.2529999999999</v>
       </c>
       <c r="E6" s="3">
         <f>D6/60</f>
-        <v>39.50438333333333</v>
+        <v>22.554216666666665</v>
       </c>
       <c r="F6" s="3">
-        <v>1359.4469999999999</v>
+        <v>833.23400000000004</v>
       </c>
       <c r="G6" s="3">
         <f>F6/60</f>
-        <v>22.657449999999997</v>
+        <v>13.887233333333334</v>
       </c>
       <c r="H6" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1">
-        <f>C4/H6</f>
-        <v>70.837940249999988</v>
+        <f>C3/H6</f>
+        <v>35.418970124999994</v>
       </c>
       <c r="J6" s="1">
-        <f>E4/H6</f>
-        <v>35.802029166666664</v>
+        <f>E3/H6</f>
+        <v>17.901014583333332</v>
       </c>
       <c r="K6" s="1">
-        <f>G4/H6</f>
-        <v>18.581766666666667</v>
+        <f>G3/H6</f>
+        <v>9.2908833333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>960</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2370.3290000000002</v>
-      </c>
-      <c r="C7" s="3">
-        <f>B7/60</f>
-        <v>39.505483333333338</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1353.2529999999999</v>
-      </c>
-      <c r="E7" s="3">
-        <f>D7/60</f>
-        <v>22.554216666666665</v>
-      </c>
-      <c r="F7" s="3">
-        <v>833.23400000000004</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7/60</f>
-        <v>13.887233333333334</v>
-      </c>
-      <c r="H7" s="1">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1">
-        <f>C4/H7</f>
-        <v>35.418970124999994</v>
-      </c>
-      <c r="J7" s="1">
-        <f>E4/H7</f>
-        <v>17.901014583333332</v>
-      </c>
-      <c r="K7" s="1">
-        <f>G4/H7</f>
-        <v>9.2908833333333334</v>
-      </c>
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="R10" s="3"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
@@ -10401,27 +9934,24 @@
     <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B60" s="4"/>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I73" s="2"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-    </row>
-    <row r="75" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
+    <row r="74" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -10433,7 +9963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66862FFB-A21C-4C47-A1F4-25D36CCA6263}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="119" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -10448,22 +9978,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -10573,22 +10103,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -10932,19 +10462,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -11179,15 +10709,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>41.045283580186599</v>
@@ -11195,7 +10725,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>30.084220517506399</v>
@@ -11203,7 +10733,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>5.4325421279670199</v>
@@ -11211,7 +10741,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>4.3116088314668799</v>
@@ -11219,7 +10749,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>3.0056241455761201</v>
@@ -11227,7 +10757,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>2.36777237085361</v>
@@ -11235,7 +10765,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>2.3505953519340999</v>
@@ -11243,7 +10773,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>1.5593899856208899</v>
@@ -11251,7 +10781,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>1.35007827053982</v>
@@ -11275,19 +10805,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -11470,15 +11000,15 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <f>17.02</f>
@@ -11490,7 +11020,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>16.580233</v>
@@ -11524,29 +11054,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>4.9578499999999996</v>
@@ -11563,7 +11093,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>11.36838333</v>

</xml_diff>